<commit_message>
Update .RData, .Rhistory, BP_JP14.svg, and 38 more files
</commit_message>
<xml_diff>
--- a/Genomes/Mirochondrial genome/Match mito genes .xlsx
+++ b/Genomes/Mirochondrial genome/Match mito genes .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0aad98ece63395da/Documentos_UFV/LAPROBQI/Genomes_S_cerevisiae_stingtless_bee/Genomes/Mirochondrial genome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{613D1AA0-37E0-4B86-A262-81BDC9210D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{613D1AA0-37E0-4B86-A262-81BDC9210D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FE30C4F-A590-420F-A5A6-CFB410F20D40}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-1308" windowWidth="23256" windowHeight="13176" xr2:uid="{E5D5612D-C55D-4CAF-8785-858FF2E079C4}"/>
   </bookViews>
@@ -625,7 +625,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>